<commit_message>
Fix one section header.
Signed-off-by: Hendriela <hendrik-heiser@gmx.de>
</commit_message>
<xml_diff>
--- a/src/data/ICHOM_PROM_breast_cancer.xlsx
+++ b/src/data/ICHOM_PROM_breast_cancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendrik\PycharmProjects\hackzurich2021\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB314568-4735-4657-B967-084C602AE65A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8882D27E-3BB0-40CE-81FF-9BCB15B21B40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$J$1:$J$998</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$J$1:$J$997</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
   <si>
     <t>Number</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Has your physical condition or medical treatment caused you financial difficulties?</t>
   </si>
   <si>
-    <t>For the following questions please circle the number between 1 and 7 that best applies to you</t>
-  </si>
-  <si>
     <t>Very Poor</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
   </si>
   <si>
     <t>Somewhat</t>
-  </si>
-  <si>
-    <t>During the past 7 days:</t>
   </si>
   <si>
     <t>I have pain in my joints</t>
@@ -600,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J998"/>
+  <dimension ref="A1:J997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -626,13 +620,13 @@
         <v>1</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -668,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -691,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -714,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -737,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -760,7 +754,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -789,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -812,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -835,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -858,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -881,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -904,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -927,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -950,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -973,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -996,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1019,7 +1013,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1042,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1065,7 +1059,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1088,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1111,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1134,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1157,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1180,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1203,7 +1197,7 @@
         <v>4</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1226,7 +1220,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1272,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1295,33 +1289,33 @@
         <v>4</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1330,7 +1324,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -1354,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1362,7 +1356,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -1386,7 +1380,7 @@
         <v>7</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1412,7 +1406,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -1427,7 +1421,7 @@
         <v>4</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1435,7 +1429,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -1450,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1458,7 +1452,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -1473,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1481,7 +1475,7 @@
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
@@ -1496,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1504,7 +1498,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
@@ -1519,7 +1513,7 @@
         <v>4</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1527,7 +1521,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
@@ -1542,7 +1536,7 @@
         <v>4</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1550,7 +1544,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
@@ -1565,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1567,7 @@
         <v>38</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1588,7 +1582,7 @@
         <v>4</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1596,7 +1590,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -1611,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1619,7 +1613,7 @@
         <v>40</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
@@ -1634,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1642,7 +1636,7 @@
         <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -1657,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1665,7 +1659,7 @@
         <v>42</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
@@ -1680,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1688,7 +1682,7 @@
         <v>43</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
@@ -1703,12 +1697,12 @@
         <v>4</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J49" s="6"/>
     </row>
@@ -1717,7 +1711,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
@@ -1732,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1740,7 +1734,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -1755,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1763,7 +1757,7 @@
         <v>46</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
@@ -1778,7 +1772,7 @@
         <v>4</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1792,7 +1786,7 @@
         <v>47</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
@@ -1807,7 +1801,7 @@
         <v>4</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1815,7 +1809,7 @@
         <v>48</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
@@ -1830,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1838,7 +1832,7 @@
         <v>49</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
@@ -1853,7 +1847,7 @@
         <v>4</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1855,7 @@
         <v>50</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
@@ -1876,7 +1870,7 @@
         <v>4</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1884,7 +1878,7 @@
         <v>51</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
@@ -1899,7 +1893,7 @@
         <v>4</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1907,7 +1901,7 @@
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="2">
         <v>1</v>
@@ -1922,7 +1916,7 @@
         <v>4</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1930,7 +1924,7 @@
         <v>53</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="2">
         <v>1</v>
@@ -1945,7 +1939,7 @@
         <v>4</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1960,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>4</v>
@@ -1975,7 +1969,7 @@
         <v>54</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2">
         <v>1</v>
@@ -1993,21 +1987,41 @@
         <v>5</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J63" s="6"/>
+      <c r="A63" s="2">
+        <v>55</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2</v>
+      </c>
+      <c r="E63" s="2">
+        <v>3</v>
+      </c>
+      <c r="F63" s="2">
+        <v>4</v>
+      </c>
+      <c r="G63" s="4">
+        <v>5</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="2">
         <v>1</v>
@@ -2025,15 +2039,15 @@
         <v>5</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -2051,15 +2065,15 @@
         <v>5</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -2077,15 +2091,15 @@
         <v>5</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67" s="2">
         <v>1</v>
@@ -2103,15 +2117,15 @@
         <v>5</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C68" s="2">
         <v>1</v>
@@ -2129,42 +2143,17 @@
         <v>5</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>60</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2">
-        <v>2</v>
-      </c>
-      <c r="E69" s="2">
-        <v>3</v>
-      </c>
-      <c r="F69" s="2">
-        <v>4</v>
-      </c>
-      <c r="G69" s="4">
-        <v>5</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="4"/>
-    </row>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3092,9 +3081,8 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="J1:J998" xr:uid="{1345FBD8-C0F5-4A2B-883D-3690EFBD1518}"/>
+  <autoFilter ref="J1:J997" xr:uid="{1345FBD8-C0F5-4A2B-883D-3690EFBD1518}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>